<commit_message>
unit one hundred thirty-nine - intermediate
</commit_message>
<xml_diff>
--- a/homework/139.xlsx
+++ b/homework/139.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{1796A2DE-CE10-4F29-B2E3-3CB75140D096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67A19CA6-7E57-41C7-900D-66050AFEC1D2}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="5910" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5670" yWindow="4770" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
   <dimension ref="A3:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C36" sqref="C34:C36"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>